<commit_message>
Updating stats with corrected data_correlations
</commit_message>
<xml_diff>
--- a/statistics/Spearmans-matrix-plots/results/Kidney-QTL-Paper/correlations and p values.xlsx
+++ b/statistics/Spearmans-matrix-plots/results/Kidney-QTL-Paper/correlations and p values.xlsx
@@ -361,27 +361,27 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Kidney GSH (nmol/mg)</t>
+          <t>Renal GSH (nmol/mg)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Kidney GSSG (nmol/mg)</t>
+          <t>Renal GSSG (nmol/mg)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Kidney Total Glutathione (nmol/mg)</t>
+          <t>Renal Total Glutathione (nmol/mg)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kidney GSH/GSSG</t>
+          <t>Renal GSH/GSSG</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Kidney Eh (mV)</t>
+          <t>Renal Eh (mV)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -391,27 +391,27 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Liver GSH (nmol/mg)</t>
+          <t>Hepatic GSH (nmol/mg)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Liver GSSG (nmol/mg)</t>
+          <t>Hepatic GSSG (nmol/mg)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Liver Total Glutathione (nmol/mg)</t>
+          <t>Hepatic Total Glutathione (nmol/mg)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Liver GSH/GSSG</t>
+          <t>Hepatic GSH/GSSG</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Liver Eh (mV)</t>
+          <t>Hepatic Eh (mV)</t>
         </is>
       </c>
     </row>
@@ -420,179 +420,179 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.3465927348859382</v>
+        <v>0.3521064146258778</v>
       </c>
       <c r="C2">
-        <v>0.9979946582745408</v>
+        <v>0.9980528573398034</v>
       </c>
       <c r="D2">
-        <v>0.4066182261417005</v>
+        <v>0.4013309999581033</v>
       </c>
       <c r="E2">
-        <v>-0.7744513428018732</v>
+        <v>-0.7732465092520669</v>
       </c>
       <c r="F2">
-        <v>0.07121445498857892</v>
+        <v>0.07121445498857891</v>
       </c>
       <c r="G2">
-        <v>0.2136143636696619</v>
+        <v>0.1989854281876762</v>
       </c>
       <c r="H2">
-        <v>0.173264429847222</v>
+        <v>0.1568556770569907</v>
       </c>
       <c r="I2">
-        <v>0.2138748776715382</v>
+        <v>0.1993024726669089</v>
       </c>
       <c r="J2">
-        <v>0.02001592346487286</v>
+        <v>0.02221124464434825</v>
       </c>
       <c r="K2">
-        <v>-0.1642862667679381</v>
+        <v>-0.1536022281255304</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.3465927348859382</v>
+        <v>0.3521064146258778</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.3893158430209376</v>
+        <v>0.394263316972649</v>
       </c>
       <c r="D3">
-        <v>-0.6597516579546294</v>
+        <v>-0.6606076551040662</v>
       </c>
       <c r="E3">
-        <v>0.2659923912469089</v>
+        <v>0.2625452042503621</v>
       </c>
       <c r="F3">
         <v>0.003355491492366705</v>
       </c>
       <c r="G3">
-        <v>-0.04422872312757233</v>
+        <v>-0.05876753207235465</v>
       </c>
       <c r="H3">
-        <v>0.03555982529662256</v>
+        <v>0.01434459480465678</v>
       </c>
       <c r="I3">
-        <v>-0.04134800991516908</v>
+        <v>-0.05602228799564749</v>
       </c>
       <c r="J3">
-        <v>-0.1256357713452548</v>
+        <v>-0.1257951259286456</v>
       </c>
       <c r="K3">
-        <v>0.09141455879115823</v>
+        <v>0.1046137714338123</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.9979946582745408</v>
+        <v>0.9980528573398034</v>
       </c>
       <c r="B4">
-        <v>0.3893158430209376</v>
+        <v>0.394263316972649</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.3650371888849235</v>
+        <v>0.3602168507545853</v>
       </c>
       <c r="E4">
-        <v>-0.7441106559630326</v>
+        <v>-0.7432812758557322</v>
       </c>
       <c r="F4">
         <v>0.06704117126479425</v>
       </c>
       <c r="G4">
-        <v>0.2075869358644635</v>
+        <v>0.1927129152134672</v>
       </c>
       <c r="H4">
-        <v>0.1713332479210322</v>
+        <v>0.1544126655825603</v>
       </c>
       <c r="I4">
-        <v>0.2080206513086957</v>
+        <v>0.1931987257790364</v>
       </c>
       <c r="J4">
-        <v>0.01247224624283352</v>
+        <v>0.01469164365969326</v>
       </c>
       <c r="K4">
-        <v>-0.1555089730616485</v>
+        <v>-0.1445993923683179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.4066182261417005</v>
+        <v>0.4013309999581033</v>
       </c>
       <c r="B5">
-        <v>-0.6597516579546294</v>
+        <v>-0.6606076551040662</v>
       </c>
       <c r="C5">
-        <v>0.3650371888849235</v>
+        <v>0.3602168507545853</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>-0.8806919197990548</v>
+        <v>-0.8790005084834919</v>
       </c>
       <c r="F5">
-        <v>0.05935148474608828</v>
+        <v>0.05935148474608827</v>
       </c>
       <c r="G5">
-        <v>0.2161774847677678</v>
+        <v>0.2185035389282103</v>
       </c>
       <c r="H5">
-        <v>0.1042931660590635</v>
+        <v>0.1124841865156832</v>
       </c>
       <c r="I5">
-        <v>0.2134119567486856</v>
+        <v>0.2158769791319677</v>
       </c>
       <c r="J5">
-        <v>0.1476489016064949</v>
+        <v>0.1497587271766938</v>
       </c>
       <c r="K5">
-        <v>-0.2215282215459371</v>
+        <v>-0.2264377540702833</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>-0.7744513428018732</v>
+        <v>-0.7732465092520669</v>
       </c>
       <c r="B6">
-        <v>0.2659923912469089</v>
+        <v>0.2625452042503621</v>
       </c>
       <c r="C6">
-        <v>-0.7441106559630326</v>
+        <v>-0.7432812758557322</v>
       </c>
       <c r="D6">
-        <v>-0.8806919197990548</v>
+        <v>-0.8790005084834919</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>-0.07916312637738217</v>
+        <v>-0.07916312637738215</v>
       </c>
       <c r="G6">
-        <v>-0.2523061884304632</v>
+        <v>-0.2462622373808689</v>
       </c>
       <c r="H6">
-        <v>-0.1494754299736874</v>
+        <v>-0.1472789699141999</v>
       </c>
       <c r="I6">
-        <v>-0.2503220438713596</v>
+        <v>-0.2444318995834648</v>
       </c>
       <c r="J6">
-        <v>-0.1231202605392072</v>
+        <v>-0.1241568421850889</v>
       </c>
       <c r="K6">
-        <v>0.2408502211283557</v>
+        <v>0.2376473570794778</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.07121445498857892</v>
+        <v>0.07121445498857891</v>
       </c>
       <c r="B7">
         <v>0.003355491492366705</v>
@@ -601,200 +601,200 @@
         <v>0.06704117126479425</v>
       </c>
       <c r="D7">
-        <v>0.05935148474608828</v>
+        <v>0.05935148474608827</v>
       </c>
       <c r="E7">
-        <v>-0.07916312637738217</v>
+        <v>-0.07916312637738215</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.1376096186459778</v>
+        <v>0.13369871861718</v>
       </c>
       <c r="H7">
-        <v>0.1015712950081312</v>
+        <v>0.09772014760320902</v>
       </c>
       <c r="I7">
-        <v>0.1349768123096158</v>
+        <v>0.1310647815837681</v>
       </c>
       <c r="J7">
-        <v>0.03616194767225479</v>
+        <v>0.03675699777175288</v>
       </c>
       <c r="K7">
-        <v>-0.1267059266331937</v>
+        <v>-0.1230157056334216</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.2136143636696619</v>
+        <v>0.1989854281876762</v>
       </c>
       <c r="B8">
-        <v>-0.04422872312757233</v>
+        <v>-0.05876753207235465</v>
       </c>
       <c r="C8">
-        <v>0.2075869358644635</v>
+        <v>0.1927129152134672</v>
       </c>
       <c r="D8">
-        <v>0.2161774847677678</v>
+        <v>0.2185035389282103</v>
       </c>
       <c r="E8">
-        <v>-0.2523061884304632</v>
+        <v>-0.2462622373808689</v>
       </c>
       <c r="F8">
-        <v>0.1376096186459778</v>
+        <v>0.13369871861718</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.7822762515495492</v>
+        <v>0.7905492366557961</v>
       </c>
       <c r="I8">
-        <v>0.9996785888277983</v>
+        <v>0.999682482891086</v>
       </c>
       <c r="J8">
-        <v>0.1491121766996026</v>
+        <v>0.1372934228397522</v>
       </c>
       <c r="K8">
-        <v>-0.8046063662189266</v>
+        <v>-0.8100036720158353</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.173264429847222</v>
+        <v>0.1568556770569907</v>
       </c>
       <c r="B9">
-        <v>0.03555982529662256</v>
+        <v>0.01434459480465678</v>
       </c>
       <c r="C9">
-        <v>0.1713332479210322</v>
+        <v>0.1544126655825603</v>
       </c>
       <c r="D9">
-        <v>0.1042931660590635</v>
+        <v>0.1124841865156832</v>
       </c>
       <c r="E9">
-        <v>-0.1494754299736874</v>
+        <v>-0.1472789699141999</v>
       </c>
       <c r="F9">
-        <v>0.1015712950081312</v>
+        <v>0.09772014760320902</v>
       </c>
       <c r="G9">
-        <v>0.7822762515495492</v>
+        <v>0.7905492366557961</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>0.7934757257736273</v>
+        <v>0.8014468546416662</v>
       </c>
       <c r="J9">
-        <v>-0.4425311946361838</v>
+        <v>-0.4429971406708035</v>
       </c>
       <c r="K9">
-        <v>-0.3068590136294691</v>
+        <v>-0.3256331147881447</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.2138748776715382</v>
+        <v>0.1993024726669089</v>
       </c>
       <c r="B10">
-        <v>-0.04134800991516908</v>
+        <v>-0.05602228799564749</v>
       </c>
       <c r="C10">
-        <v>0.2080206513086957</v>
+        <v>0.1931987257790364</v>
       </c>
       <c r="D10">
-        <v>0.2134119567486856</v>
+        <v>0.2158769791319677</v>
       </c>
       <c r="E10">
-        <v>-0.2503220438713596</v>
+        <v>-0.2444318995834648</v>
       </c>
       <c r="F10">
-        <v>0.1349768123096158</v>
+        <v>0.1310647815837681</v>
       </c>
       <c r="G10">
-        <v>0.9996785888277983</v>
+        <v>0.999682482891086</v>
       </c>
       <c r="H10">
-        <v>0.7934757257736273</v>
+        <v>0.8014468546416662</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0.1316914367088446</v>
+        <v>0.12005681992252</v>
       </c>
       <c r="K10">
-        <v>-0.7933256565835511</v>
+        <v>-0.7989592333815935</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.02001592346487286</v>
+        <v>0.02221124464434825</v>
       </c>
       <c r="B11">
-        <v>-0.1256357713452548</v>
+        <v>-0.1257951259286456</v>
       </c>
       <c r="C11">
-        <v>0.01247224624283352</v>
+        <v>0.01469164365969326</v>
       </c>
       <c r="D11">
-        <v>0.1476489016064949</v>
+        <v>0.1497587271766938</v>
       </c>
       <c r="E11">
-        <v>-0.1231202605392072</v>
+        <v>-0.1241568421850889</v>
       </c>
       <c r="F11">
-        <v>0.03616194767225479</v>
+        <v>0.03675699777175288</v>
       </c>
       <c r="G11">
-        <v>0.1491121766996026</v>
+        <v>0.1372934228397522</v>
       </c>
       <c r="H11">
-        <v>-0.4425311946361838</v>
+        <v>-0.4429971406708035</v>
       </c>
       <c r="I11">
-        <v>0.1316914367088446</v>
+        <v>0.12005681992252</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
-        <v>-0.6682039148421686</v>
+        <v>-0.6524132569486403</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-0.1642862667679381</v>
+        <v>-0.1536022281255304</v>
       </c>
       <c r="B12">
-        <v>0.09141455879115823</v>
+        <v>0.1046137714338123</v>
       </c>
       <c r="C12">
-        <v>-0.1555089730616485</v>
+        <v>-0.1445993923683179</v>
       </c>
       <c r="D12">
-        <v>-0.2215282215459371</v>
+        <v>-0.2264377540702833</v>
       </c>
       <c r="E12">
-        <v>0.2408502211283557</v>
+        <v>0.2376473570794778</v>
       </c>
       <c r="F12">
-        <v>-0.1267059266331937</v>
+        <v>-0.1230157056334216</v>
       </c>
       <c r="G12">
-        <v>-0.8046063662189266</v>
+        <v>-0.8100036720158353</v>
       </c>
       <c r="H12">
-        <v>-0.3068590136294691</v>
+        <v>-0.3256331147881447</v>
       </c>
       <c r="I12">
-        <v>-0.7933256565835511</v>
+        <v>-0.7989592333815935</v>
       </c>
       <c r="J12">
-        <v>-0.6682039148421686</v>
+        <v>-0.6524132569486403</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -816,27 +816,27 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Kidney GSH (nmol/mg)</t>
+          <t>Renal GSH (nmol/mg)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Kidney GSSG (nmol/mg)</t>
+          <t>Renal GSSG (nmol/mg)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Kidney Total Glutathione (nmol/mg)</t>
+          <t>Renal Total Glutathione (nmol/mg)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kidney GSH/GSSG</t>
+          <t>Renal GSH/GSSG</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Kidney Eh (mV)</t>
+          <t>Renal Eh (mV)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -846,27 +846,27 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Liver GSH (nmol/mg)</t>
+          <t>Hepatic GSH (nmol/mg)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Liver GSSG (nmol/mg)</t>
+          <t>Hepatic GSSG (nmol/mg)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Liver Total Glutathione (nmol/mg)</t>
+          <t>Hepatic Total Glutathione (nmol/mg)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Liver GSH/GSSG</t>
+          <t>Hepatic GSH/GSSG</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Liver Eh (mV)</t>
+          <t>Hepatic Eh (mV)</t>
         </is>
       </c>
     </row>

</xml_diff>